<commit_message>
Scrum board and Scrum Master Log
</commit_message>
<xml_diff>
--- a/Project/Scrum board.xlsx
+++ b/Project/Scrum board.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\ganttproject\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B560614-EB6B-4BEA-922A-2C70F168620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976FD5EC-873B-4BF6-A0FE-5F49CF873E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBEFE5C5-46DB-4AFD-85F6-E2741116B6AB}"/>
   </bookViews>
@@ -35,9 +35,65 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Create fork for GanttProject (Daniel)</t>
+  </si>
+  <si>
+    <t>Clone branch repo (all)</t>
+  </si>
+  <si>
+    <t>Make GantProject run locally (all)</t>
+  </si>
+  <si>
+    <t>Find 3 code patterns (all)</t>
+  </si>
+  <si>
+    <t>Find 3 code smells (all)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Reviewing</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Create User Stories - All</t>
+  </si>
+  <si>
+    <t>Analize the program to find possible User Stories - All</t>
+  </si>
+  <si>
+    <t>Discuss possible implementations - All</t>
+  </si>
+  <si>
+    <t>Identify key structures - All</t>
+  </si>
+  <si>
+    <t>Analize the Metrics - All</t>
+  </si>
+  <si>
+    <t>Implementação do código - All</t>
+  </si>
+  <si>
+    <t>Criação dos use Cases - All</t>
+  </si>
+  <si>
+    <t>Criação e Análise das Métricas - All</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +101,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -62,14 +143,213 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Ênfase6" xfId="2" builtinId="50"/>
+    <cellStyle name="Ênfase6" xfId="1" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,12 +662,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4CC099-578A-4323-B44F-145954CB311A}">
-  <dimension ref="A1"/>
+  <dimension ref="E2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="8" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>